<commit_message>
New tle and xlsx files added to validation. Validation results updated for software v1.2
</commit_message>
<xml_diff>
--- a/gs_files/gs_2.xlsx
+++ b/gs_files/gs_2.xlsx
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +442,7 @@
     <col min="11" max="13" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,147 +450,131 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>50.002464260759197</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29.5606346924565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5.1481174223964601</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-95.088395130234403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>15</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>10</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="4">
         <v>1550000000</v>
       </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>20</v>
       </c>
-      <c r="C17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>